<commit_message>
changed the groups to run in testng xml file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData_Magento.xlsx
+++ b/src/test/resources/excel/TestData_Magento.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="201">
   <si>
     <t>EditAccountPageTest</t>
   </si>
@@ -587,6 +587,45 @@
   </si>
   <si>
     <t>,,000051821,000051826,000051828,000051830</t>
+  </si>
+  <si>
+    <t>Ahluwalia D D</t>
+  </si>
+  <si>
+    <t>Sucheta Ahluwalia D D</t>
+  </si>
+  <si>
+    <t>,,000051821,000051826,000051828,000051830,</t>
+  </si>
+  <si>
+    <t>xjeic@gmail.com</t>
+  </si>
+  <si>
+    <t>U9h49w153@</t>
+  </si>
+  <si>
+    <t>Nalini</t>
+  </si>
+  <si>
+    <t>Nalini Sethi</t>
+  </si>
+  <si>
+    <t>Sethi D</t>
+  </si>
+  <si>
+    <t>Nalini Sethi D</t>
+  </si>
+  <si>
+    <t>Sethi D D</t>
+  </si>
+  <si>
+    <t>Nalini Sethi D D</t>
+  </si>
+  <si>
+    <t>,,</t>
+  </si>
+  <si>
+    <t>,,,000052964</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1076,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD9"/>
@@ -1611,13 +1650,33 @@
         <v>179</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="E33" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the pom file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData_Magento.xlsx
+++ b/src/test/resources/excel/TestData_Magento.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="216">
   <si>
     <t>EditAccountPageTest</t>
   </si>
@@ -626,6 +626,51 @@
   </si>
   <si>
     <t>,,,000052964</t>
+  </si>
+  <si>
+    <t>Sethi D D D</t>
+  </si>
+  <si>
+    <t>Nalini Sethi D D D</t>
+  </si>
+  <si>
+    <t>,,,000052964,</t>
+  </si>
+  <si>
+    <t>unzoq@gmail.com</t>
+  </si>
+  <si>
+    <t>3Eflpr385@</t>
+  </si>
+  <si>
+    <t>Vidhur</t>
+  </si>
+  <si>
+    <t>Chopra</t>
+  </si>
+  <si>
+    <t>Vidhur Chopra</t>
+  </si>
+  <si>
+    <t>fsjol@gmail.com</t>
+  </si>
+  <si>
+    <t>PE9vzx758^</t>
+  </si>
+  <si>
+    <t>Urmila</t>
+  </si>
+  <si>
+    <t>Talwar</t>
+  </si>
+  <si>
+    <t>Urmila Talwar</t>
+  </si>
+  <si>
+    <t>Talwar D</t>
+  </si>
+  <si>
+    <t>Urmila Talwar D</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1121,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD9"/>
@@ -1670,13 +1715,51 @@
         <v>193</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="E33" t="s" s="0">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>204</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>207</v>
+      </c>
+      <c r="E34" t="s" s="0">
+        <v>208</v>
+      </c>
+      <c r="F34" s="0"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>209</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>210</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>211</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="E35" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the extentreport in ExtentManager
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData_Magento.xlsx
+++ b/src/test/resources/excel/TestData_Magento.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="235">
   <si>
     <t>EditAccountPageTest</t>
   </si>
@@ -671,6 +671,63 @@
   </si>
   <si>
     <t>Urmila Talwar D</t>
+  </si>
+  <si>
+    <t>firwl@gmail.com</t>
+  </si>
+  <si>
+    <t>1Aemst205^</t>
+  </si>
+  <si>
+    <t>Karthik</t>
+  </si>
+  <si>
+    <t>Agarwal</t>
+  </si>
+  <si>
+    <t>Karthik Agarwal</t>
+  </si>
+  <si>
+    <t>Agarwal D</t>
+  </si>
+  <si>
+    <t>Karthik Agarwal D</t>
+  </si>
+  <si>
+    <t>bmzim@gmail.com</t>
+  </si>
+  <si>
+    <t>T4bekl736*</t>
+  </si>
+  <si>
+    <t>Bhadraksh</t>
+  </si>
+  <si>
+    <t>Bhadraksh Kapoor</t>
+  </si>
+  <si>
+    <t>Kapoor D</t>
+  </si>
+  <si>
+    <t>Bhadraksh Kapoor D</t>
+  </si>
+  <si>
+    <t>dclob@gmail.com</t>
+  </si>
+  <si>
+    <t>KCn62l343!</t>
+  </si>
+  <si>
+    <t>Pothuvaal</t>
+  </si>
+  <si>
+    <t>Shubha Pothuvaal</t>
+  </si>
+  <si>
+    <t>Pothuvaal D</t>
+  </si>
+  <si>
+    <t>Shubha Pothuvaal D</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1178,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD9"/>
@@ -1762,6 +1819,66 @@
         <v>166</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>216</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>217</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>218</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>221</v>
+      </c>
+      <c r="E36" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>223</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>224</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>225</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>227</v>
+      </c>
+      <c r="E37" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>229</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>233</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upgraded the selenium version
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData_Magento.xlsx
+++ b/src/test/resources/excel/TestData_Magento.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="268">
   <si>
     <t>EditAccountPageTest</t>
   </si>
@@ -806,6 +806,27 @@
   </si>
   <si>
     <t>Brahmanandam Panicker D</t>
+  </si>
+  <si>
+    <t>fittd@gmail.com</t>
+  </si>
+  <si>
+    <t>SUu6bq349$</t>
+  </si>
+  <si>
+    <t>Birjesh</t>
+  </si>
+  <si>
+    <t>Bandopadhyay</t>
+  </si>
+  <si>
+    <t>Birjesh Bandopadhyay</t>
+  </si>
+  <si>
+    <t>Bandopadhyay D</t>
+  </si>
+  <si>
+    <t>Birjesh Bandopadhyay D</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1277,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD9"/>
@@ -2035,6 +2056,26 @@
         <v>166</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>262</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>266</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>267</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>